<commit_message>
Cleanued up some unnecessary highlights
</commit_message>
<xml_diff>
--- a/v1 ETL/flyersdbmodel.xlsx
+++ b/v1 ETL/flyersdbmodel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2f59d8c8ae45d7d/Documents/BI Git/v1 ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{BE6E66BA-3035-4CA9-9069-08B3CB23BC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC7B019C-3863-4E7C-9CCC-247AEFA50920}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{BE6E66BA-3035-4CA9-9069-08B3CB23BC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE05B118-5DCE-4FC8-B10A-A12BFAE31D85}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" activeTab="1" xr2:uid="{BBADE8C8-DEB0-43F4-8CBE-BB05BCDA3388}"/>
   </bookViews>
@@ -709,183 +709,6 @@
     <t>Distinct Count of GeneralProduct</t>
   </si>
   <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Blueberries', NULL, 'Produce', 'Blueberries', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '18oz', NULL, NULL, '2.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Simple Truth', 'Organic Blueberries', NULL, 'Produce', 'Blueberries', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', 'Unknown', '2', NULL, '3';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Honeycrisp Apples', NULL, 'Produce', 'Apples', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '1.49';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Organic Honeycrisp Apples', NULL, 'Produce', 'Apples', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '2.49';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'T-Bone Steaks', NULL, 'Meat &amp; Seafood', 'T-Bone Steaks', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '6.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Colossal Shrimp', NULL, 'Meat &amp; Seafood', 'Shrimp', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '13-15ct', NULL, NULL, '6.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Wild-Caught Alaska Whole Sockeye Salmon', NULL, 'Meat &amp; Seafood', 'Salmon', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '4.77';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Green Seedless Grapes', NULL, 'Produce', 'Grapes', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '1.68';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Tillamook', 'Cheese', NULL, 'Dairy &amp; Eggs', 'Cheese', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '32oz', '2', '4', '5.97';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Campbell''s', 'Chunky Soup', NULL, 'Canned &amp; Packaged', 'Chunky Soup', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18.6oz-19oz', '8', NULL, '0.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cottonelle', 'ComfortCare Mega Rolls Toilet Paper', NULL, 'Paper Plastics', 'Toilet Paper', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12ct', '5', NULL, '11.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Viva', 'Multi Surface Cloth Double Rolls Paper Towels', NULL, 'Paper Plastics', 'Paper Towels', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8ct', '5', NULL, '11.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cascade', 'Complete Action Pacs Select Varieties', NULL, 'Cleaning Products', 'Dishwasher Detergent', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '36-60ct', '5', NULL, '11.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'General Mills', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8.9oz-12oz', '5', NULL, '1.79';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kellogg''s', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10.1oz-18oz', '5', NULL, '1.79';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cap''n Crunch', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.5-13oz', '5', NULL, '1.79';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Life', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.5-13oz', '5', NULL, '1.79';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Dreyer''s', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '48oz', '5', NULL, '2.49';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Breyers', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '48oz', '5', NULL, '2.49';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Haagen-Dazs', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '14oz', '5', NULL, '2.49';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Haagen-Dazs', 'Ice Cream Bar', NULL, 'Frozen', 'Ice Cream Bar', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '3ct', '5', NULL, '2.49';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Green Mountain', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Donut Shop', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'McCafe', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Green Mountain', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Donut Shop', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'McCafe', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Yuban', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '22-31oz', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Gevalia', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Gevalia', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6-12ct', '5', NULL, '5.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Samsung', '65" Smart 4K Crystal Ultra HDTV (UN65TU7000)', NULL, 'Electronics', 'TV', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '597.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Chefman', '3.5-Liter Manual Air Fryer', NULL, 'Kitchen', 'Air Fryer', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '59.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Ashley', 'Kaden 40" Recliner', NULL, 'Furniture', 'Recliner', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '399.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', '80% Lean Ground Beef Patties', NULL, 'Meat &amp; Seafood', 'Ground Beef', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '10ct, 2.2lbs', NULL, NULL, '10';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Simple Truth', 'Pistachios', NULL, 'Snacks', 'Pistachios', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8oz', '2', NULL, '3.5';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Digiorno', 'Frozen Pizza', NULL, 'Frozen', 'Frozen Pizza', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18.7-31.5oz', '2', NULL, '10';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Lay''s', 'Potato Chips', NULL, 'Snacks', 'Potato Chips', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '4.75-8oz', '4', NULL, '1.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Doritos', 'Potato Chips', NULL, 'Snacks', 'Potato Chips', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6-10.75oz', '4', NULL, '1.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Tostitos', 'Tortilla Chips', NULL, 'Snacks', 'Tortilla Chips', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-13oz', '4', NULL, '1.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Michelob Ultra', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kona', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Shock Top', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Frozen Chicken Breasts', NULL, 'Meat &amp; Seafood', 'Frozen Chicken Breasts', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '3lb', NULL, '5', '5.97';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Eggs', NULL, 'Dairy &amp; Eggs', 'Eggs', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '18ct', NULL, '5', '1.27';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Oreo', 'Cookies', NULL, 'Snacks', 'Cookies', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '7.9-15.35oz', NULL, '5', '2.47';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Honey Maid', 'Graham Crackers', NULL, 'Snacks', 'Graham Crackers', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.2-14.4oz', NULL, '5', '2.47';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Freschetta', 'Frozen Pizza', NULL, 'Frozen', 'Frozen Pizza', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '17.71oz-30.88oz', NULL, '5', '3.77';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Hershey''s', 'Candy', NULL, 'Snacks', 'Candy', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '31.36-48.29oz', NULL, '5', '6.97';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Reese''s', 'Candy', NULL, 'Snacks', 'Candy', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '31.36-48.29oz', NULL, '5', '6.97';</t>
-  </si>
-  <si>
-    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Toilet Paper', NULL, 'Paper Plastics', 'Toilet Paper', 'https://flyers.blob.core.windows.net/flyerblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18ct', NULL, '5', '10.97';</t>
-  </si>
-  <si>
     <t>White Claw</t>
   </si>
   <si>
@@ -1076,6 +899,183 @@
   </si>
   <si>
     <t>https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Blueberries', NULL, 'Produce', 'Blueberries', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '18oz', NULL, NULL, '2.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Simple Truth', 'Organic Blueberries', NULL, 'Produce', 'Blueberries', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', 'Unknown', '2', NULL, '3';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Honeycrisp Apples', NULL, 'Produce', 'Apples', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '1.49';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Organic Honeycrisp Apples', NULL, 'Produce', 'Apples', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '2.49';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'T-Bone Steaks', NULL, 'Meat &amp; Seafood', 'T-Bone Steaks', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '6.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Colossal Shrimp', NULL, 'Meat &amp; Seafood', 'Shrimp', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '13-15ct', NULL, NULL, '6.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Wild-Caught Alaska Whole Sockeye Salmon', NULL, 'Meat &amp; Seafood', 'Salmon', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '4.77';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Green Seedless Grapes', NULL, 'Produce', 'Grapes', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '1.68';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Tillamook', 'Cheese', NULL, 'Dairy &amp; Eggs', 'Cheese', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '32oz', '2', '4', '5.97';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Campbell''s', 'Soup', NULL, 'Canned &amp; Packaged', 'Soup', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18.6oz-19oz', '8', NULL, '0.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cottonelle', 'ComfortCare Mega Rolls Toilet Paper', NULL, 'Paper Plastics', 'Toilet Paper', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12ct', '5', NULL, '11.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Viva', 'Multi Surface Cloth Double Rolls Paper Towels', NULL, 'Paper Plastics', 'Paper Towels', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8ct', '5', NULL, '11.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cascade', 'Complete Action Pacs Select Varieties', NULL, 'Cleaning Products', 'Dishwasher Detergent', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '36-60ct', '5', NULL, '11.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'General Mills', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8.9oz-12oz', '5', NULL, '1.79';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kellogg''s', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10.1oz-18oz', '5', NULL, '1.79';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cap''n Crunch', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.5-13oz', '5', NULL, '1.79';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Life', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.5-13oz', '5', NULL, '1.79';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Dreyer''s', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '48oz', '5', NULL, '2.49';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Breyers', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '48oz', '5', NULL, '2.49';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Haagen-Dazs', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '14oz', '5', NULL, '2.49';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Haagen-Dazs', 'Ice Cream Bar', NULL, 'Frozen', 'Ice Cream Bar', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '3ct', '5', NULL, '2.49';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Green Mountain', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Donut Shop', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'McCafe', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Green Mountain', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Donut Shop', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'McCafe', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Yuban', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '22-31oz', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Gevalia', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Gevalia', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6-12ct', '5', NULL, '5.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Samsung', '65" Smart 4K Crystal Ultra HDTV (UN65TU7000)', NULL, 'Electronics', 'TV', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '597.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Chefman', '3.5-Liter Manual Air Fryer', NULL, 'Kitchen', 'Air Fryer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '59.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Ashley', 'Kaden 40" Recliner', NULL, 'Furniture', 'Recliner', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '399.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', '80% Lean Ground Beef Patties', NULL, 'Meat &amp; Seafood', 'Ground Beef', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '10ct, 2.2lbs', NULL, NULL, '10';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Simple Truth', 'Pistachios', NULL, 'Snacks', 'Pistachios', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8oz', '2', NULL, '3.5';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Digiorno', 'Frozen Pizza', NULL, 'Frozen', 'Frozen Pizza', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18.7-31.5oz', '2', NULL, '10';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Lay''s', 'Potato Chips', NULL, 'Snacks', 'Potato Chips', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '4.75-8oz', '4', NULL, '1.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Doritos', 'Potato Chips', NULL, 'Snacks', 'Potato Chips', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6-10.75oz', '4', NULL, '1.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Tostitos', 'Tortilla Chips', NULL, 'Snacks', 'Tortilla Chips', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-13oz', '4', NULL, '1.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Michelob Ultra', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kona', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Shock Top', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Frozen Chicken Breasts', NULL, 'Meat &amp; Seafood', 'Frozen Chicken Breasts', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '3lb', NULL, '5', '5.97';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Eggs', NULL, 'Dairy &amp; Eggs', 'Eggs', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '18ct', NULL, '5', '1.27';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Oreo', 'Cookies', NULL, 'Snacks', 'Cookies', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '7.9-15.35oz', NULL, '5', '2.47';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Honey Maid', 'Graham Crackers', NULL, 'Snacks', 'Graham Crackers', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.2-14.4oz', NULL, '5', '2.47';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Freschetta', 'Frozen Pizza', NULL, 'Frozen', 'Frozen Pizza', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '17.71oz-30.88oz', NULL, '5', '3.77';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Hershey''s', 'Candy', NULL, 'Snacks', 'Candy', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '31.36-48.29oz', NULL, '5', '6.97';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Reese''s', 'Candy', NULL, 'Snacks', 'Candy', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '31.36-48.29oz', NULL, '5', '6.97';</t>
+  </si>
+  <si>
+    <t>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Toilet Paper', NULL, 'Paper Plastics', 'Toilet Paper', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18ct', NULL, '5', '10.97';</t>
   </si>
 </sst>
 </file>
@@ -1099,24 +1099,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -1160,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1172,13 +1160,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1785,6 +1766,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2821,7 +2806,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>269</v>
+        <v>210</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2863,7 +2848,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3199,7 +3184,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -3262,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E96FF6-1DC4-49AA-883E-6A0DFAF568E6}">
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3340,43 +3325,43 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>329</v>
-      </c>
-      <c r="I2" s="14">
-        <v>44587</v>
-      </c>
-      <c r="J2" s="14">
-        <v>44593</v>
-      </c>
-      <c r="K2" s="14" t="s">
+      <c r="H2" t="s">
+        <v>270</v>
+      </c>
+      <c r="I2" s="5">
+        <v>44587</v>
+      </c>
+      <c r="J2" s="5">
+        <v>44593</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="15">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="6">
         <v>2.99</v>
       </c>
       <c r="Q2" t="str">
@@ -3384,7 +3369,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Blueberries', NULL, 'Produce', 'Blueberries', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '18oz', NULL, NULL, '2.99';</v>
       </c>
       <c r="R2" t="s">
-        <v>207</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -3407,8 +3392,8 @@
       <c r="G3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>329</v>
+      <c r="H3" t="s">
+        <v>270</v>
       </c>
       <c r="I3" s="5">
         <v>44587</v>
@@ -3434,7 +3419,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Simple Truth', 'Organic Blueberries', NULL, 'Produce', 'Blueberries', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', 'Unknown', '2', NULL, '3';</v>
       </c>
       <c r="R3" t="s">
-        <v>208</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -3457,8 +3442,8 @@
       <c r="G4" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>329</v>
+      <c r="H4" t="s">
+        <v>270</v>
       </c>
       <c r="I4" s="5">
         <v>44587</v>
@@ -3482,7 +3467,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Honeycrisp Apples', NULL, 'Produce', 'Apples', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '1.49';</v>
       </c>
       <c r="R4" t="s">
-        <v>209</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -3505,8 +3490,8 @@
       <c r="G5" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>329</v>
+      <c r="H5" t="s">
+        <v>270</v>
       </c>
       <c r="I5" s="5">
         <v>44587</v>
@@ -3530,7 +3515,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Organic Honeycrisp Apples', NULL, 'Produce', 'Apples', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '2.49';</v>
       </c>
       <c r="R5" t="s">
-        <v>210</v>
+        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -3553,8 +3538,8 @@
       <c r="G6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="11" t="s">
-        <v>329</v>
+      <c r="H6" t="s">
+        <v>270</v>
       </c>
       <c r="I6" s="5">
         <v>44587</v>
@@ -3578,7 +3563,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'T-Bone Steaks', NULL, 'Meat &amp; Seafood', 'T-Bone Steaks', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '6.99';</v>
       </c>
       <c r="R6" t="s">
-        <v>211</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -3601,8 +3586,8 @@
       <c r="G7" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>329</v>
+      <c r="H7" t="s">
+        <v>270</v>
       </c>
       <c r="I7" s="5">
         <v>44587</v>
@@ -3626,7 +3611,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Colossal Shrimp', NULL, 'Meat &amp; Seafood', 'Shrimp', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '13-15ct', NULL, NULL, '6.99';</v>
       </c>
       <c r="R7" t="s">
-        <v>212</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -3649,8 +3634,8 @@
       <c r="G8" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>329</v>
+      <c r="H8" t="s">
+        <v>270</v>
       </c>
       <c r="I8" s="5">
         <v>44587</v>
@@ -3674,7 +3659,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Wild-Caught Alaska Whole Sockeye Salmon', NULL, 'Meat &amp; Seafood', 'Salmon', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '4.77';</v>
       </c>
       <c r="R8" t="s">
-        <v>213</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -3697,8 +3682,8 @@
       <c r="G9" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>329</v>
+      <c r="H9" t="s">
+        <v>270</v>
       </c>
       <c r="I9" s="5">
         <v>44587</v>
@@ -3722,7 +3707,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Fred Meyer', 'Green Seedless Grapes', NULL, 'Produce', 'Grapes', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1lb', NULL, NULL, '1.68';</v>
       </c>
       <c r="R9" t="s">
-        <v>214</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3745,8 +3730,8 @@
       <c r="G10" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H10" s="11" t="s">
-        <v>329</v>
+      <c r="H10" t="s">
+        <v>270</v>
       </c>
       <c r="I10" s="5">
         <v>44587</v>
@@ -3772,7 +3757,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</v>
       </c>
       <c r="R10" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -3795,8 +3780,8 @@
       <c r="G11" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>329</v>
+      <c r="H11" t="s">
+        <v>270</v>
       </c>
       <c r="I11" s="5">
         <v>44587</v>
@@ -3822,7 +3807,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</v>
       </c>
       <c r="R11" t="s">
-        <v>216</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -3845,8 +3830,8 @@
       <c r="G12" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>329</v>
+      <c r="H12" t="s">
+        <v>270</v>
       </c>
       <c r="I12" s="5">
         <v>44587</v>
@@ -3872,7 +3857,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6ct (16.9oz or 7.5oz)', '4', NULL, '3';</v>
       </c>
       <c r="R12" t="s">
-        <v>217</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -3895,8 +3880,8 @@
       <c r="G13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>329</v>
+      <c r="H13" t="s">
+        <v>270</v>
       </c>
       <c r="I13" s="5">
         <v>44587</v>
@@ -3924,7 +3909,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Tillamook', 'Cheese', NULL, 'Dairy &amp; Eggs', 'Cheese', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '32oz', '2', '4', '5.97';</v>
       </c>
       <c r="R13" t="s">
-        <v>218</v>
+        <v>282</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -3938,17 +3923,17 @@
         <v>141</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>318</v>
+        <v>259</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
         <v>165</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>329</v>
+        <v>259</v>
+      </c>
+      <c r="H14" t="s">
+        <v>270</v>
       </c>
       <c r="I14" s="5">
         <v>44587</v>
@@ -3974,7 +3959,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Campbell''s', 'Soup', NULL, 'Canned &amp; Packaged', 'Soup', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18.6oz-19oz', '8', NULL, '0.99';</v>
       </c>
       <c r="R14" t="s">
-        <v>219</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -3997,8 +3982,8 @@
       <c r="G15" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H15" s="11" t="s">
-        <v>329</v>
+      <c r="H15" t="s">
+        <v>270</v>
       </c>
       <c r="I15" s="5">
         <v>44587</v>
@@ -4024,7 +4009,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cottonelle', 'ComfortCare Mega Rolls Toilet Paper', NULL, 'Paper Plastics', 'Toilet Paper', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12ct', '5', NULL, '11.99';</v>
       </c>
       <c r="R15" t="s">
-        <v>220</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -4047,8 +4032,8 @@
       <c r="G16" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H16" s="11" t="s">
-        <v>329</v>
+      <c r="H16" t="s">
+        <v>270</v>
       </c>
       <c r="I16" s="5">
         <v>44587</v>
@@ -4074,7 +4059,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Viva', 'Multi Surface Cloth Double Rolls Paper Towels', NULL, 'Paper Plastics', 'Paper Towels', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8ct', '5', NULL, '11.99';</v>
       </c>
       <c r="R16" t="s">
-        <v>221</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -4097,8 +4082,8 @@
       <c r="G17" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="H17" s="11" t="s">
-        <v>329</v>
+      <c r="H17" t="s">
+        <v>270</v>
       </c>
       <c r="I17" s="5">
         <v>44587</v>
@@ -4124,7 +4109,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cascade', 'Complete Action Pacs Select Varieties', NULL, 'Cleaning Products', 'Dishwasher Detergent', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '36-60ct', '5', NULL, '11.99';</v>
       </c>
       <c r="R17" t="s">
-        <v>222</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -4147,8 +4132,8 @@
       <c r="G18" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>329</v>
+      <c r="H18" t="s">
+        <v>270</v>
       </c>
       <c r="I18" s="5">
         <v>44587</v>
@@ -4174,7 +4159,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'General Mills', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8.9oz-12oz', '5', NULL, '1.79';</v>
       </c>
       <c r="R18" t="s">
-        <v>223</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
@@ -4197,8 +4182,8 @@
       <c r="G19" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>329</v>
+      <c r="H19" t="s">
+        <v>270</v>
       </c>
       <c r="I19" s="5">
         <v>44587</v>
@@ -4224,7 +4209,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kellogg''s', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10.1oz-18oz', '5', NULL, '1.79';</v>
       </c>
       <c r="R19" t="s">
-        <v>224</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -4247,8 +4232,8 @@
       <c r="G20" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H20" s="11" t="s">
-        <v>329</v>
+      <c r="H20" t="s">
+        <v>270</v>
       </c>
       <c r="I20" s="5">
         <v>44587</v>
@@ -4274,7 +4259,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Cap''n Crunch', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.5-13oz', '5', NULL, '1.79';</v>
       </c>
       <c r="R20" t="s">
-        <v>225</v>
+        <v>289</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -4297,8 +4282,8 @@
       <c r="G21" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>329</v>
+      <c r="H21" t="s">
+        <v>270</v>
       </c>
       <c r="I21" s="5">
         <v>44587</v>
@@ -4324,7 +4309,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Life', 'Cereal', NULL, 'Breakfast', 'Cereal', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.5-13oz', '5', NULL, '1.79';</v>
       </c>
       <c r="R21" t="s">
-        <v>226</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -4347,8 +4332,8 @@
       <c r="G22" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>329</v>
+      <c r="H22" t="s">
+        <v>270</v>
       </c>
       <c r="I22" s="5">
         <v>44587</v>
@@ -4374,7 +4359,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Dreyer''s', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '48oz', '5', NULL, '2.49';</v>
       </c>
       <c r="R22" t="s">
-        <v>227</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -4397,8 +4382,8 @@
       <c r="G23" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>329</v>
+      <c r="H23" t="s">
+        <v>270</v>
       </c>
       <c r="I23" s="5">
         <v>44587</v>
@@ -4424,7 +4409,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Breyers', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '48oz', '5', NULL, '2.49';</v>
       </c>
       <c r="R23" t="s">
-        <v>228</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -4447,8 +4432,8 @@
       <c r="G24" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>329</v>
+      <c r="H24" t="s">
+        <v>270</v>
       </c>
       <c r="I24" s="5">
         <v>44587</v>
@@ -4474,7 +4459,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Haagen-Dazs', 'Ice Cream', NULL, 'Frozen', 'Ice Cream', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '14oz', '5', NULL, '2.49';</v>
       </c>
       <c r="R24" t="s">
-        <v>229</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -4497,8 +4482,8 @@
       <c r="G25" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>329</v>
+      <c r="H25" t="s">
+        <v>270</v>
       </c>
       <c r="I25" s="5">
         <v>44587</v>
@@ -4524,7 +4509,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Haagen-Dazs', 'Ice Cream Bar', NULL, 'Frozen', 'Ice Cream Bar', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '3ct', '5', NULL, '2.49';</v>
       </c>
       <c r="R25" t="s">
-        <v>230</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -4547,8 +4532,8 @@
       <c r="G26" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>329</v>
+      <c r="H26" t="s">
+        <v>270</v>
       </c>
       <c r="I26" s="5">
         <v>44587</v>
@@ -4574,7 +4559,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Green Mountain', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</v>
       </c>
       <c r="R26" t="s">
-        <v>231</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
@@ -4597,8 +4582,8 @@
       <c r="G27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>329</v>
+      <c r="H27" t="s">
+        <v>270</v>
       </c>
       <c r="I27" s="5">
         <v>44587</v>
@@ -4624,7 +4609,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Donut Shop', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</v>
       </c>
       <c r="R27" t="s">
-        <v>232</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -4647,8 +4632,8 @@
       <c r="G28" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>329</v>
+      <c r="H28" t="s">
+        <v>270</v>
       </c>
       <c r="I28" s="5">
         <v>44587</v>
@@ -4674,7 +4659,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'McCafe', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</v>
       </c>
       <c r="R28" t="s">
-        <v>233</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -4697,8 +4682,8 @@
       <c r="G29" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H29" s="11" t="s">
-        <v>329</v>
+      <c r="H29" t="s">
+        <v>270</v>
       </c>
       <c r="I29" s="5">
         <v>44587</v>
@@ -4724,7 +4709,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Green Mountain', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</v>
       </c>
       <c r="R29" t="s">
-        <v>234</v>
+        <v>298</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -4747,8 +4732,8 @@
       <c r="G30" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H30" s="11" t="s">
-        <v>329</v>
+      <c r="H30" t="s">
+        <v>270</v>
       </c>
       <c r="I30" s="5">
         <v>44587</v>
@@ -4774,7 +4759,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Donut Shop', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</v>
       </c>
       <c r="R30" t="s">
-        <v>235</v>
+        <v>299</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -4797,8 +4782,8 @@
       <c r="G31" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H31" s="11" t="s">
-        <v>329</v>
+      <c r="H31" t="s">
+        <v>270</v>
       </c>
       <c r="I31" s="5">
         <v>44587</v>
@@ -4824,7 +4809,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'McCafe', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-12ct', '5', NULL, '5.99';</v>
       </c>
       <c r="R31" t="s">
-        <v>236</v>
+        <v>300</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -4847,8 +4832,8 @@
       <c r="G32" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="H32" s="11" t="s">
-        <v>329</v>
+      <c r="H32" t="s">
+        <v>270</v>
       </c>
       <c r="I32" s="5">
         <v>44587</v>
@@ -4874,7 +4859,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Yuban', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '22-31oz', '5', NULL, '5.99';</v>
       </c>
       <c r="R32" t="s">
-        <v>237</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
@@ -4897,8 +4882,8 @@
       <c r="G33" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="H33" s="11" t="s">
-        <v>329</v>
+      <c r="H33" t="s">
+        <v>270</v>
       </c>
       <c r="I33" s="5">
         <v>44587</v>
@@ -4924,7 +4909,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Gevalia', 'Coffee', NULL, 'Beverages', 'Coffee', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10oz-12oz', '5', NULL, '5.99';</v>
       </c>
       <c r="R33" t="s">
-        <v>238</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
@@ -4947,8 +4932,8 @@
       <c r="G34" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="H34" s="11" t="s">
-        <v>329</v>
+      <c r="H34" t="s">
+        <v>270</v>
       </c>
       <c r="I34" s="5">
         <v>44587</v>
@@ -4974,7 +4959,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Gevalia', 'K-Cups', NULL, 'Beverages', 'K-Cups', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6-12ct', '5', NULL, '5.99';</v>
       </c>
       <c r="R34" t="s">
-        <v>239</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
@@ -4997,8 +4982,8 @@
       <c r="G35" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H35" s="11" t="s">
-        <v>329</v>
+      <c r="H35" t="s">
+        <v>270</v>
       </c>
       <c r="I35" s="5">
         <v>44587</v>
@@ -5022,7 +5007,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Samsung', '65" Smart 4K Crystal Ultra HDTV (UN65TU7000)', NULL, 'Electronics', 'TV', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '597.99';</v>
       </c>
       <c r="R35" t="s">
-        <v>240</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
@@ -5045,8 +5030,8 @@
       <c r="G36" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="H36" s="11" t="s">
-        <v>329</v>
+      <c r="H36" t="s">
+        <v>270</v>
       </c>
       <c r="I36" s="5">
         <v>44587</v>
@@ -5070,7 +5055,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Chefman', '3.5-Liter Manual Air Fryer', NULL, 'Kitchen', 'Air Fryer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '59.99';</v>
       </c>
       <c r="R36" t="s">
-        <v>241</v>
+        <v>305</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -5093,8 +5078,8 @@
       <c r="G37" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="H37" s="11" t="s">
-        <v>329</v>
+      <c r="H37" t="s">
+        <v>270</v>
       </c>
       <c r="I37" s="5">
         <v>44587</v>
@@ -5118,7 +5103,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Ashley', 'Kaden 40" Recliner', NULL, 'Furniture', 'Recliner', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '1ct', NULL, NULL, '399.99';</v>
       </c>
       <c r="R37" t="s">
-        <v>242</v>
+        <v>306</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -5141,8 +5126,8 @@
       <c r="G38" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>329</v>
+      <c r="H38" t="s">
+        <v>270</v>
       </c>
       <c r="I38" s="5">
         <v>44587</v>
@@ -5166,7 +5151,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', '80% Lean Ground Beef Patties', NULL, 'Meat &amp; Seafood', 'Ground Beef', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '10ct, 2.2lbs', NULL, NULL, '10';</v>
       </c>
       <c r="R38" t="s">
-        <v>243</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
@@ -5189,8 +5174,8 @@
       <c r="G39" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>329</v>
+      <c r="H39" t="s">
+        <v>270</v>
       </c>
       <c r="I39" s="5">
         <v>44587</v>
@@ -5216,7 +5201,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Simple Truth', 'Pistachios', NULL, 'Snacks', 'Pistachios', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8oz', '2', NULL, '3.5';</v>
       </c>
       <c r="R39" t="s">
-        <v>244</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
@@ -5239,8 +5224,8 @@
       <c r="G40" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>329</v>
+      <c r="H40" t="s">
+        <v>270</v>
       </c>
       <c r="I40" s="5">
         <v>44587</v>
@@ -5266,7 +5251,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Digiorno', 'Frozen Pizza', NULL, 'Frozen', 'Frozen Pizza', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18.7-31.5oz', '2', NULL, '10';</v>
       </c>
       <c r="R40" t="s">
-        <v>245</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
@@ -5289,8 +5274,8 @@
       <c r="G41" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="H41" s="11" t="s">
-        <v>329</v>
+      <c r="H41" t="s">
+        <v>270</v>
       </c>
       <c r="I41" s="5">
         <v>44587</v>
@@ -5316,7 +5301,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Lay''s', 'Potato Chips', NULL, 'Snacks', 'Potato Chips', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '4.75-8oz', '4', NULL, '1.99';</v>
       </c>
       <c r="R41" t="s">
-        <v>246</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
@@ -5339,8 +5324,8 @@
       <c r="G42" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="H42" s="11" t="s">
-        <v>329</v>
+      <c r="H42" t="s">
+        <v>270</v>
       </c>
       <c r="I42" s="5">
         <v>44587</v>
@@ -5366,7 +5351,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Doritos', 'Potato Chips', NULL, 'Snacks', 'Potato Chips', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '6-10.75oz', '4', NULL, '1.99';</v>
       </c>
       <c r="R42" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -5389,8 +5374,8 @@
       <c r="G43" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="H43" s="11" t="s">
-        <v>329</v>
+      <c r="H43" t="s">
+        <v>270</v>
       </c>
       <c r="I43" s="5">
         <v>44587</v>
@@ -5416,7 +5401,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Tostitos', 'Tortilla Chips', NULL, 'Snacks', 'Tortilla Chips', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '10-13oz', '4', NULL, '1.99';</v>
       </c>
       <c r="R43" t="s">
-        <v>248</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -5439,8 +5424,8 @@
       <c r="G44" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H44" s="11" t="s">
-        <v>329</v>
+      <c r="H44" t="s">
+        <v>270</v>
       </c>
       <c r="I44" s="5">
         <v>44587</v>
@@ -5466,7 +5451,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</v>
       </c>
       <c r="R44" t="s">
-        <v>249</v>
+        <v>313</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -5489,8 +5474,8 @@
       <c r="G45" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H45" s="11" t="s">
-        <v>329</v>
+      <c r="H45" t="s">
+        <v>270</v>
       </c>
       <c r="I45" s="5">
         <v>44587</v>
@@ -5516,7 +5501,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</v>
       </c>
       <c r="R45" t="s">
-        <v>250</v>
+        <v>314</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
@@ -5539,8 +5524,8 @@
       <c r="G46" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>329</v>
+      <c r="H46" t="s">
+        <v>270</v>
       </c>
       <c r="I46" s="5">
         <v>44587</v>
@@ -5566,7 +5551,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', '3', NULL, '4.33';</v>
       </c>
       <c r="R46" t="s">
-        <v>251</v>
+        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
@@ -5589,8 +5574,8 @@
       <c r="G47" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H47" s="11" t="s">
-        <v>329</v>
+      <c r="H47" t="s">
+        <v>270</v>
       </c>
       <c r="I47" s="5">
         <v>44587</v>
@@ -5616,7 +5601,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Coca-Cola', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</v>
       </c>
       <c r="R47" t="s">
-        <v>252</v>
+        <v>316</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -5639,8 +5624,8 @@
       <c r="G48" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H48" s="11" t="s">
-        <v>329</v>
+      <c r="H48" t="s">
+        <v>270</v>
       </c>
       <c r="I48" s="5">
         <v>44587</v>
@@ -5666,7 +5651,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Pepsi', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</v>
       </c>
       <c r="R48" t="s">
-        <v>253</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
@@ -5689,8 +5674,8 @@
       <c r="G49" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="H49" s="11" t="s">
-        <v>329</v>
+      <c r="H49" t="s">
+        <v>270</v>
       </c>
       <c r="I49" s="5">
         <v>44587</v>
@@ -5716,7 +5701,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Seven Up', 'Soda', NULL, 'Beverages', 'Soda', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '8-pack of 12oz', '3', NULL, '4.33';</v>
       </c>
       <c r="R49" t="s">
-        <v>254</v>
+        <v>318</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
@@ -5739,8 +5724,8 @@
       <c r="G50" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H50" s="11" t="s">
-        <v>329</v>
+      <c r="H50" t="s">
+        <v>270</v>
       </c>
       <c r="I50" s="5">
         <v>44587</v>
@@ -5764,7 +5749,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Michelob Ultra', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</v>
       </c>
       <c r="R50" t="s">
-        <v>255</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
@@ -5787,8 +5772,8 @@
       <c r="G51" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H51" s="11" t="s">
-        <v>329</v>
+      <c r="H51" t="s">
+        <v>270</v>
       </c>
       <c r="I51" s="5">
         <v>44587</v>
@@ -5812,7 +5797,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kona', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</v>
       </c>
       <c r="R51" t="s">
-        <v>256</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
@@ -5835,8 +5820,8 @@
       <c r="G52" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H52" s="11" t="s">
-        <v>329</v>
+      <c r="H52" t="s">
+        <v>270</v>
       </c>
       <c r="I52" s="5">
         <v>44587</v>
@@ -5860,7 +5845,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Shock Top', 'Beer', NULL, 'Adult Beverage', 'Beer', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12-pack of 12oz', NULL, NULL, '15.99';</v>
       </c>
       <c r="R52" t="s">
-        <v>257</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
@@ -5883,8 +5868,8 @@
       <c r="G53" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H53" s="11" t="s">
-        <v>329</v>
+      <c r="H53" t="s">
+        <v>270</v>
       </c>
       <c r="I53" s="5">
         <v>44587</v>
@@ -5910,7 +5895,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Frozen Chicken Breasts', NULL, 'Meat &amp; Seafood', 'Frozen Chicken Breasts', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '3lb', NULL, '5', '5.97';</v>
       </c>
       <c r="R53" t="s">
-        <v>258</v>
+        <v>322</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
@@ -5933,8 +5918,8 @@
       <c r="G54" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="H54" s="11" t="s">
-        <v>329</v>
+      <c r="H54" t="s">
+        <v>270</v>
       </c>
       <c r="I54" s="5">
         <v>44587</v>
@@ -5960,7 +5945,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Eggs', NULL, 'Dairy &amp; Eggs', 'Eggs', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Specific', '18ct', NULL, '5', '1.27';</v>
       </c>
       <c r="R54" t="s">
-        <v>259</v>
+        <v>323</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
@@ -5983,8 +5968,8 @@
       <c r="G55" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="H55" s="11" t="s">
-        <v>329</v>
+      <c r="H55" t="s">
+        <v>270</v>
       </c>
       <c r="I55" s="5">
         <v>44587</v>
@@ -6010,7 +5995,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Oreo', 'Cookies', NULL, 'Snacks', 'Cookies', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '7.9-15.35oz', NULL, '5', '2.47';</v>
       </c>
       <c r="R55" t="s">
-        <v>260</v>
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
@@ -6033,8 +6018,8 @@
       <c r="G56" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H56" s="11" t="s">
-        <v>329</v>
+      <c r="H56" t="s">
+        <v>270</v>
       </c>
       <c r="I56" s="5">
         <v>44587</v>
@@ -6060,7 +6045,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Honey Maid', 'Graham Crackers', NULL, 'Snacks', 'Graham Crackers', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '12.2-14.4oz', NULL, '5', '2.47';</v>
       </c>
       <c r="R56" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
@@ -6083,8 +6068,8 @@
       <c r="G57" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="H57" s="11" t="s">
-        <v>329</v>
+      <c r="H57" t="s">
+        <v>270</v>
       </c>
       <c r="I57" s="5">
         <v>44587</v>
@@ -6110,7 +6095,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Freschetta', 'Frozen Pizza', NULL, 'Frozen', 'Frozen Pizza', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '17.71oz-30.88oz', NULL, '5', '3.77';</v>
       </c>
       <c r="R57" t="s">
-        <v>262</v>
+        <v>326</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
@@ -6133,8 +6118,8 @@
       <c r="G58" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="H58" s="11" t="s">
-        <v>329</v>
+      <c r="H58" t="s">
+        <v>270</v>
       </c>
       <c r="I58" s="5">
         <v>44587</v>
@@ -6160,7 +6145,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Hershey''s', 'Candy', NULL, 'Snacks', 'Candy', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '31.36-48.29oz', NULL, '5', '6.97';</v>
       </c>
       <c r="R58" t="s">
-        <v>263</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
@@ -6183,8 +6168,8 @@
       <c r="G59" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="H59" s="11" t="s">
-        <v>329</v>
+      <c r="H59" t="s">
+        <v>270</v>
       </c>
       <c r="I59" s="5">
         <v>44587</v>
@@ -6210,7 +6195,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Reese''s', 'Candy', NULL, 'Snacks', 'Candy', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '31.36-48.29oz', NULL, '5', '6.97';</v>
       </c>
       <c r="R59" t="s">
-        <v>264</v>
+        <v>328</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
@@ -6233,8 +6218,8 @@
       <c r="G60" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="H60" s="11" t="s">
-        <v>329</v>
+      <c r="H60" t="s">
+        <v>270</v>
       </c>
       <c r="I60" s="5">
         <v>44587</v>
@@ -6260,7 +6245,7 @@
         <v>exec InsertNormalizedAd 'Grocery', 'Fred Meyer', 'Kroger', 'Toilet Paper', NULL, 'Paper Plastics', 'Toilet Paper', 'https://flyersstorage.blob.core.windows.net/flyersblobs/FM20220126.pdf', '2022-01-26', '2022-02-01', 'Variety', '18ct', NULL, '5', '10.97';</v>
       </c>
       <c r="R60" t="s">
-        <v>265</v>
+        <v>329</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
@@ -6271,20 +6256,20 @@
         <v>3</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>266</v>
+        <v>207</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>269</v>
+        <v>210</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>329</v>
+        <v>210</v>
+      </c>
+      <c r="H61" t="s">
+        <v>270</v>
       </c>
       <c r="I61" s="5">
         <v>44587</v>
@@ -6312,20 +6297,20 @@
         <v>3</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>267</v>
+        <v>208</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>269</v>
+        <v>210</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>329</v>
+        <v>210</v>
+      </c>
+      <c r="H62" t="s">
+        <v>270</v>
       </c>
       <c r="I62" s="5">
         <v>44587</v>
@@ -6353,20 +6338,20 @@
         <v>3</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>268</v>
+        <v>209</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>269</v>
+        <v>210</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>329</v>
+        <v>210</v>
+      </c>
+      <c r="H63" t="s">
+        <v>270</v>
       </c>
       <c r="I63" s="5">
         <v>44587</v>
@@ -6394,7 +6379,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>270</v>
+        <v>211</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>195</v>
@@ -6406,8 +6391,8 @@
       <c r="G64" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H64" s="11" t="s">
-        <v>329</v>
+      <c r="H64" t="s">
+        <v>270</v>
       </c>
       <c r="I64" s="5">
         <v>44587</v>
@@ -6435,7 +6420,7 @@
         <v>3</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>271</v>
+        <v>212</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>195</v>
@@ -6447,8 +6432,8 @@
       <c r="G65" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H65" s="11" t="s">
-        <v>329</v>
+      <c r="H65" t="s">
+        <v>270</v>
       </c>
       <c r="I65" s="5">
         <v>44587</v>
@@ -6460,7 +6445,7 @@
         <v>150</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>272</v>
+        <v>213</v>
       </c>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
@@ -6476,7 +6461,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>273</v>
+        <v>214</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>195</v>
@@ -6488,8 +6473,8 @@
       <c r="G66" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H66" s="11" t="s">
-        <v>329</v>
+      <c r="H66" t="s">
+        <v>270</v>
       </c>
       <c r="I66" s="5">
         <v>44587</v>
@@ -6501,7 +6486,7 @@
         <v>150</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
@@ -6517,7 +6502,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>274</v>
+        <v>215</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>195</v>
@@ -6529,8 +6514,8 @@
       <c r="G67" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H67" s="11" t="s">
-        <v>329</v>
+      <c r="H67" t="s">
+        <v>270</v>
       </c>
       <c r="I67" s="5">
         <v>44587</v>
@@ -6542,7 +6527,7 @@
         <v>150</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
@@ -6558,7 +6543,7 @@
         <v>3</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>275</v>
+        <v>216</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>195</v>
@@ -6570,8 +6555,8 @@
       <c r="G68" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H68" s="11" t="s">
-        <v>329</v>
+      <c r="H68" t="s">
+        <v>270</v>
       </c>
       <c r="I68" s="5">
         <v>44587</v>
@@ -6583,7 +6568,7 @@
         <v>150</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
@@ -6599,7 +6584,7 @@
         <v>3</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>276</v>
+        <v>217</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>195</v>
@@ -6611,8 +6596,8 @@
       <c r="G69" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H69" s="11" t="s">
-        <v>329</v>
+      <c r="H69" t="s">
+        <v>270</v>
       </c>
       <c r="I69" s="5">
         <v>44587</v>
@@ -6624,7 +6609,7 @@
         <v>150</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
@@ -6640,7 +6625,7 @@
         <v>3</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>278</v>
+        <v>219</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>195</v>
@@ -6652,8 +6637,8 @@
       <c r="G70" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H70" s="11" t="s">
-        <v>329</v>
+      <c r="H70" t="s">
+        <v>270</v>
       </c>
       <c r="I70" s="5">
         <v>44587</v>
@@ -6665,7 +6650,7 @@
         <v>150</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
@@ -6681,7 +6666,7 @@
         <v>3</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>270</v>
+        <v>211</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>195</v>
@@ -6693,8 +6678,8 @@
       <c r="G71" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H71" s="11" t="s">
-        <v>329</v>
+      <c r="H71" t="s">
+        <v>270</v>
       </c>
       <c r="I71" s="5">
         <v>44587</v>
@@ -6706,7 +6691,7 @@
         <v>150</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
@@ -6722,7 +6707,7 @@
         <v>3</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>279</v>
+        <v>220</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>195</v>
@@ -6734,8 +6719,8 @@
       <c r="G72" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H72" s="11" t="s">
-        <v>329</v>
+      <c r="H72" t="s">
+        <v>270</v>
       </c>
       <c r="I72" s="5">
         <v>44587</v>
@@ -6747,7 +6732,7 @@
         <v>150</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>277</v>
+        <v>218</v>
       </c>
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
@@ -6763,20 +6748,20 @@
         <v>3</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>280</v>
+        <v>221</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H73" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H73" t="s">
+        <v>270</v>
       </c>
       <c r="I73" s="5">
         <v>44587</v>
@@ -6788,7 +6773,7 @@
         <v>150</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
@@ -6804,20 +6789,20 @@
         <v>3</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>281</v>
+        <v>222</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H74" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H74" t="s">
+        <v>270</v>
       </c>
       <c r="I74" s="5">
         <v>44587</v>
@@ -6829,7 +6814,7 @@
         <v>150</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
@@ -6845,20 +6830,20 @@
         <v>3</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>282</v>
+        <v>223</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H75" t="s">
+        <v>270</v>
       </c>
       <c r="I75" s="5">
         <v>44587</v>
@@ -6870,7 +6855,7 @@
         <v>150</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
@@ -6886,20 +6871,20 @@
         <v>3</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>283</v>
+        <v>224</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H76" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H76" t="s">
+        <v>270</v>
       </c>
       <c r="I76" s="5">
         <v>44587</v>
@@ -6911,7 +6896,7 @@
         <v>150</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
@@ -6927,20 +6912,20 @@
         <v>3</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>286</v>
+        <v>227</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H77" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H77" t="s">
+        <v>270</v>
       </c>
       <c r="I77" s="5">
         <v>44587</v>
@@ -6952,7 +6937,7 @@
         <v>150</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
@@ -6968,20 +6953,20 @@
         <v>3</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>287</v>
+        <v>228</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H78" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H78" t="s">
+        <v>270</v>
       </c>
       <c r="I78" s="5">
         <v>44587</v>
@@ -6993,7 +6978,7 @@
         <v>150</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
@@ -7009,20 +6994,20 @@
         <v>3</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>288</v>
+        <v>229</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H79" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H79" t="s">
+        <v>270</v>
       </c>
       <c r="I79" s="5">
         <v>44587</v>
@@ -7034,7 +7019,7 @@
         <v>150</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M79" s="4"/>
       <c r="N79" s="4"/>
@@ -7050,20 +7035,20 @@
         <v>3</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>289</v>
+        <v>230</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H80" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H80" t="s">
+        <v>270</v>
       </c>
       <c r="I80" s="5">
         <v>44587</v>
@@ -7075,7 +7060,7 @@
         <v>150</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>290</v>
+        <v>231</v>
       </c>
       <c r="M80" s="4"/>
       <c r="N80" s="4"/>
@@ -7091,20 +7076,20 @@
         <v>3</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>291</v>
+        <v>232</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H81" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H81" t="s">
+        <v>270</v>
       </c>
       <c r="I81" s="5">
         <v>44587</v>
@@ -7116,7 +7101,7 @@
         <v>150</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M81" s="4"/>
       <c r="N81" s="4"/>
@@ -7132,20 +7117,20 @@
         <v>3</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>292</v>
+        <v>233</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H82" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H82" t="s">
+        <v>270</v>
       </c>
       <c r="I82" s="5">
         <v>44587</v>
@@ -7157,7 +7142,7 @@
         <v>150</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M82" s="4"/>
       <c r="N82" s="4"/>
@@ -7173,20 +7158,20 @@
         <v>3</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>293</v>
+        <v>234</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>284</v>
+        <v>225</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="H83" s="11" t="s">
-        <v>329</v>
+        <v>225</v>
+      </c>
+      <c r="H83" t="s">
+        <v>270</v>
       </c>
       <c r="I83" s="5">
         <v>44587</v>
@@ -7198,7 +7183,7 @@
         <v>150</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
@@ -7214,20 +7199,20 @@
         <v>3</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>294</v>
+        <v>235</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H84" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H84" t="s">
+        <v>270</v>
       </c>
       <c r="I84" s="5">
         <v>44587</v>
@@ -7239,7 +7224,7 @@
         <v>150</v>
       </c>
       <c r="L84" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M84" s="4"/>
       <c r="N84" s="4"/>
@@ -7255,20 +7240,20 @@
         <v>3</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>295</v>
+        <v>236</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H85" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H85" t="s">
+        <v>270</v>
       </c>
       <c r="I85" s="5">
         <v>44587</v>
@@ -7280,7 +7265,7 @@
         <v>150</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M85" s="4"/>
       <c r="N85" s="4"/>
@@ -7296,20 +7281,20 @@
         <v>3</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>296</v>
+        <v>237</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H86" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H86" t="s">
+        <v>270</v>
       </c>
       <c r="I86" s="5">
         <v>44587</v>
@@ -7321,7 +7306,7 @@
         <v>150</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
@@ -7337,20 +7322,20 @@
         <v>3</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>297</v>
+        <v>238</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H87" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H87" t="s">
+        <v>270</v>
       </c>
       <c r="I87" s="5">
         <v>44587</v>
@@ -7362,7 +7347,7 @@
         <v>150</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
@@ -7378,20 +7363,20 @@
         <v>3</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>299</v>
+        <v>240</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H88" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H88" t="s">
+        <v>270</v>
       </c>
       <c r="I88" s="5">
         <v>44587</v>
@@ -7403,7 +7388,7 @@
         <v>150</v>
       </c>
       <c r="L88" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
@@ -7419,20 +7404,20 @@
         <v>3</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>300</v>
+        <v>241</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H89" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H89" t="s">
+        <v>270</v>
       </c>
       <c r="I89" s="5">
         <v>44587</v>
@@ -7444,7 +7429,7 @@
         <v>150</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
@@ -7460,20 +7445,20 @@
         <v>3</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>301</v>
+        <v>242</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H90" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H90" t="s">
+        <v>270</v>
       </c>
       <c r="I90" s="5">
         <v>44587</v>
@@ -7485,7 +7470,7 @@
         <v>150</v>
       </c>
       <c r="L90" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
@@ -7501,20 +7486,20 @@
         <v>3</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>302</v>
+        <v>243</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H91" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H91" t="s">
+        <v>270</v>
       </c>
       <c r="I91" s="5">
         <v>44587</v>
@@ -7526,7 +7511,7 @@
         <v>150</v>
       </c>
       <c r="L91" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
@@ -7542,20 +7527,20 @@
         <v>3</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>303</v>
+        <v>244</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H92" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H92" t="s">
+        <v>270</v>
       </c>
       <c r="I92" s="5">
         <v>44587</v>
@@ -7567,7 +7552,7 @@
         <v>150</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
@@ -7583,20 +7568,20 @@
         <v>3</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>304</v>
+        <v>245</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H93" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H93" t="s">
+        <v>270</v>
       </c>
       <c r="I93" s="5">
         <v>44587</v>
@@ -7608,7 +7593,7 @@
         <v>150</v>
       </c>
       <c r="L93" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
@@ -7624,20 +7609,20 @@
         <v>3</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>305</v>
+        <v>246</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H94" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H94" t="s">
+        <v>270</v>
       </c>
       <c r="I94" s="5">
         <v>44587</v>
@@ -7649,7 +7634,7 @@
         <v>150</v>
       </c>
       <c r="L94" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M94" s="4"/>
       <c r="N94" s="4"/>
@@ -7665,20 +7650,20 @@
         <v>3</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>306</v>
+        <v>247</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H95" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H95" t="s">
+        <v>270</v>
       </c>
       <c r="I95" s="5">
         <v>44587</v>
@@ -7690,7 +7675,7 @@
         <v>150</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M95" s="4"/>
       <c r="N95" s="4"/>
@@ -7706,20 +7691,20 @@
         <v>3</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>307</v>
+        <v>248</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H96" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H96" t="s">
+        <v>270</v>
       </c>
       <c r="I96" s="5">
         <v>44587</v>
@@ -7731,7 +7716,7 @@
         <v>150</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
@@ -7747,20 +7732,20 @@
         <v>3</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>308</v>
+        <v>249</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H97" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H97" t="s">
+        <v>270</v>
       </c>
       <c r="I97" s="5">
         <v>44587</v>
@@ -7772,7 +7757,7 @@
         <v>150</v>
       </c>
       <c r="L97" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M97" s="4"/>
       <c r="N97" s="4"/>
@@ -7788,20 +7773,20 @@
         <v>3</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>309</v>
+        <v>250</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H98" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H98" t="s">
+        <v>270</v>
       </c>
       <c r="I98" s="5">
         <v>44587</v>
@@ -7813,7 +7798,7 @@
         <v>150</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
@@ -7829,20 +7814,20 @@
         <v>3</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>310</v>
+        <v>251</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>298</v>
+        <v>239</v>
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
         <v>174</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="H99" s="11" t="s">
-        <v>329</v>
+        <v>239</v>
+      </c>
+      <c r="H99" t="s">
+        <v>270</v>
       </c>
       <c r="I99" s="5">
         <v>44587</v>
@@ -7854,7 +7839,7 @@
         <v>150</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>285</v>
+        <v>226</v>
       </c>
       <c r="M99" s="4"/>
       <c r="N99" s="4"/>
@@ -7873,7 +7858,7 @@
         <v>3</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>311</v>
+        <v>252</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
@@ -7882,8 +7867,8 @@
       <c r="G100" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="H100" s="11" t="s">
-        <v>329</v>
+      <c r="H100" t="s">
+        <v>270</v>
       </c>
       <c r="I100" s="5">
         <v>44587</v>
@@ -7895,7 +7880,7 @@
         <v>149</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>312</v>
+        <v>253</v>
       </c>
       <c r="M100" s="4"/>
       <c r="N100" s="4">
@@ -7913,20 +7898,20 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>313</v>
+        <v>254</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>314</v>
+        <v>255</v>
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="4" t="s">
         <v>173</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H101" s="11" t="s">
-        <v>329</v>
+        <v>255</v>
+      </c>
+      <c r="H101" t="s">
+        <v>270</v>
       </c>
       <c r="I101" s="5">
         <v>44587</v>
@@ -7938,7 +7923,7 @@
         <v>150</v>
       </c>
       <c r="L101" s="4" t="s">
-        <v>315</v>
+        <v>256</v>
       </c>
       <c r="M101" s="4"/>
       <c r="N101" s="4">
@@ -7956,20 +7941,20 @@
         <v>3</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>316</v>
+        <v>257</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>317</v>
+        <v>258</v>
       </c>
       <c r="E102" s="4"/>
       <c r="F102" s="4" t="s">
-        <v>319</v>
+        <v>260</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="H102" s="11" t="s">
-        <v>329</v>
+        <v>258</v>
+      </c>
+      <c r="H102" t="s">
+        <v>270</v>
       </c>
       <c r="I102" s="5">
         <v>44587</v>
@@ -7981,7 +7966,7 @@
         <v>150</v>
       </c>
       <c r="L102" s="4" t="s">
-        <v>320</v>
+        <v>261</v>
       </c>
       <c r="M102" s="4"/>
       <c r="N102" s="4">
@@ -7999,20 +7984,20 @@
         <v>3</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>322</v>
+        <v>263</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>318</v>
+        <v>259</v>
       </c>
       <c r="E103" s="4"/>
       <c r="F103" s="4" t="s">
         <v>165</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="H103" s="11" t="s">
-        <v>329</v>
+        <v>259</v>
+      </c>
+      <c r="H103" t="s">
+        <v>270</v>
       </c>
       <c r="I103" s="5">
         <v>44587</v>
@@ -8024,7 +8009,7 @@
         <v>150</v>
       </c>
       <c r="L103" s="4" t="s">
-        <v>321</v>
+        <v>262</v>
       </c>
       <c r="M103" s="4"/>
       <c r="N103" s="4">
@@ -8042,20 +8027,20 @@
         <v>3</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>322</v>
+        <v>263</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>323</v>
+        <v>264</v>
       </c>
       <c r="E104" s="4"/>
       <c r="F104" s="4" t="s">
-        <v>324</v>
+        <v>265</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="H104" s="11" t="s">
-        <v>329</v>
+        <v>264</v>
+      </c>
+      <c r="H104" t="s">
+        <v>270</v>
       </c>
       <c r="I104" s="5">
         <v>44587</v>
@@ -8067,7 +8052,7 @@
         <v>150</v>
       </c>
       <c r="L104" s="4" t="s">
-        <v>325</v>
+        <v>266</v>
       </c>
       <c r="M104" s="4"/>
       <c r="N104" s="4">
@@ -8085,20 +8070,20 @@
         <v>3</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>326</v>
+        <v>267</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>327</v>
+        <v>268</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
         <v>162</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="H105" s="11" t="s">
-        <v>329</v>
+        <v>268</v>
+      </c>
+      <c r="H105" t="s">
+        <v>270</v>
       </c>
       <c r="I105" s="5">
         <v>44587</v>
@@ -8110,7 +8095,7 @@
         <v>150</v>
       </c>
       <c r="L105" s="4" t="s">
-        <v>328</v>
+        <v>269</v>
       </c>
       <c r="M105" s="4"/>
       <c r="N105" s="4">

</xml_diff>